<commit_message>
FIX: Minor description change
</commit_message>
<xml_diff>
--- a/dah_foerstekontakt_v100_export.xlsx
+++ b/dah_foerstekontakt_v100_export.xlsx
@@ -488,17 +488,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Contact</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>NoteType</t>
+          <t>RespiratoryRate</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Første afsluttet lægenotat</t>
+          <t>Første respirationsfrekvens måling.</t>
         </is>
       </c>
     </row>
@@ -513,11 +513,6 @@
           <t>str</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Dato for første afsluttet lægenotat</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
@@ -532,17 +527,17 @@
     <row r="4">
       <c r="D4" t="inlineStr">
         <is>
-          <t>Note</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>String</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Notattype for første afsluttet lægenotat</t>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -559,12 +554,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>OxygenSaturation</t>
+          <t>PulseRate</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Første iltmætningsmåling.</t>
+          <t>Første pulsmåling.</t>
         </is>
       </c>
     </row>
@@ -598,17 +593,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Float</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Enhed = %</t>
+          <t>Integer</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
+          <t>Greater than or equal to: 0</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -625,29 +615,34 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RespiratoryRate</t>
+          <t>PainEvaluation</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Første respirationsfrekvens måling.</t>
+          <t>Første smertemåling.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="D9" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Se webservice dokumentation.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t xml:space="preserve">Enums/Udfald: | "vas" | "nrs" | "vrs" | "andet" | </t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -659,122 +654,122 @@
     <row r="10">
       <c r="D10" t="inlineStr">
         <is>
+          <t>DateTime</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" t="inlineStr">
+        <is>
           <t>ResultValue</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Float</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Værdi for smertescore</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>Greater than or equal to: 0</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>SystolicBloodPressure</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Blodtryksmåling (systolisk).</t>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="D12" t="inlineStr">
         <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Bruges ved 'andet' type af smertescore</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SystolicBloodPressure</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Første systoliske blodtryksmåling</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" t="inlineStr">
+        <is>
           <t>DateTime</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>str</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>PainEvaluation</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Første smertemåling.</t>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="D15" t="inlineStr">
         <is>
-          <t>ResultCode</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Se webservice dokumentation.</t>
+          <t>Integer</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "vas" | "nrs" | "vrs" | "andet" | </t>
+          <t>Greater than or equal to: 0</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -784,46 +779,36 @@
       </c>
     </row>
     <row r="16">
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>DateTime</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>True</t>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>OxygenDemand</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Første iltbehov.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="D17" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Float</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Værdi for smertescore</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0</t>
+          <t xml:space="preserve">Enums/Udfald: | "y" | "n" | </t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -835,17 +820,22 @@
     <row r="18">
       <c r="D18" t="inlineStr">
         <is>
-          <t>Note</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>String</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Bruges ved 'andet' type af smertescore</t>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
@@ -857,29 +847,29 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>GlasgowComaScale</t>
+          <t>AVPUScale</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Første Glasgow Coma Scale måling.</t>
+          <t>Første AVPU skala</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="D20" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t xml:space="preserve">Enums/Udfald: | "a" | "v" | "p" | "u" | </t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -891,17 +881,17 @@
     <row r="21">
       <c r="D21" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Integer</t>
+          <t>str</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 3 | Less than or equal to: 15</t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -918,29 +908,29 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Triage</t>
+          <t>GlasgowComaScale</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Første Triage kategorisering.</t>
+          <t>Første Glasgow Coma Scale måling.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
         <is>
-          <t>ResultCode</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>str, Enum</t>
+          <t>str</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "r" | "o" | "y" | "g" | "b" | </t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -952,17 +942,17 @@
     <row r="24">
       <c r="D24" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>Integer</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t>Greater than or equal to: 3 | Less than or equal to: 15</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -979,12 +969,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>AVPUScale</t>
+          <t>Triage</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Første AVPU skala</t>
+          <t>Første Triage kategorisering.</t>
         </is>
       </c>
     </row>
@@ -1001,7 +991,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "a" | "v" | "p" | "u" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "r" | "o" | "y" | "g" | "b" | </t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1106,12 +1096,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>PulseRate</t>
+          <t>OxygenSaturation</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Første pulsmåling.</t>
+          <t>Første iltmætningsmåling.</t>
         </is>
       </c>
     </row>
@@ -1145,12 +1135,17 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Integer</t>
+          <t>Float</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Enhed = %</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0</t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1162,34 +1157,39 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Contact</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>OxygenDemand</t>
+          <t>NoteType</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Første iltbehov.</t>
+          <t>Første afsluttet lægenotat</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="D35" t="inlineStr">
         <is>
-          <t>ResultCode</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>str, Enum</t>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Dato for første afsluttet lægenotat</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "y" | "n" | </t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1201,17 +1201,17 @@
     <row r="36">
       <c r="D36" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>Note</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Notattype for første afsluttet lægenotat</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">

</xml_diff>